<commit_message>
Aggiornato file con Budget Schedule Variance
</commit_message>
<xml_diff>
--- a/SWE/Documentazione/Piano_di_Progetto/file sorgenti/BVSV.xlsx
+++ b/SWE/Documentazione/Piano_di_Progetto/file sorgenti/BVSV.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\ApertureProject\SWE\Documentazione\Piano_di_Progetto\file sorgenti\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -11,13 +16,12 @@
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>norme di progetto</t>
   </si>
@@ -125,6 +129,18 @@
   </si>
   <si>
     <t>resp</t>
+  </si>
+  <si>
+    <t>man_utente</t>
+  </si>
+  <si>
+    <t>Codifica</t>
+  </si>
+  <si>
+    <t>Verifica</t>
+  </si>
+  <si>
+    <t>def prod</t>
   </si>
 </sst>
 </file>
@@ -178,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -187,6 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -197,6 +216,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -245,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,7 +302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P32"/>
+  <dimension ref="B2:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -692,7 +714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -710,7 +732,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -721,7 +743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -732,7 +754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -756,7 +778,7 @@
         <v>3686</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -764,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>20</v>
       </c>
@@ -780,8 +802,11 @@
       <c r="K23">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>14</v>
       </c>
@@ -802,20 +827,23 @@
         <v>35</v>
       </c>
       <c r="L24" s="6"/>
-      <c r="M24" t="s">
+      <c r="M24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24" t="s">
         <v>33</v>
       </c>
-      <c r="N24" t="s">
-        <v>10</v>
-      </c>
-      <c r="O24" s="4" t="s">
+      <c r="P24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P24" s="5" t="s">
+      <c r="R24" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>33</v>
       </c>
@@ -846,9 +874,15 @@
       <c r="L25" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="4"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -882,23 +916,23 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26">
+      <c r="O26">
         <f>C26*$C$23+E26*$E$23+G26*$G$23+I26*$I$23+K26*$K$23</f>
         <v>190</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <f>(C26+D26)*$C$23+(E26+F26)*$E$23+(G26+H26)*$G$23+(I26+J26)*$I$23+(K26+L26)*$K$23</f>
         <v>145</v>
       </c>
-      <c r="O26" s="4">
-        <f>M26-N26</f>
+      <c r="Q26" s="4">
+        <f>O26-P26</f>
         <v>45</v>
       </c>
-      <c r="P26">
+      <c r="R26">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
@@ -932,23 +966,23 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="M27">
-        <f t="shared" ref="M27:M31" si="1">C27*$C$23+E27*$E$23+G27*$G$23+I27*$I$23+K27*$K$23</f>
+      <c r="O27">
+        <f>C27*$C$23+E27*$E$23+G27*$G$23+I27*$I$23+K27*$K$23</f>
         <v>395</v>
       </c>
-      <c r="N27">
-        <f t="shared" ref="N27:N31" si="2">(C27+D27)*$C$23+(E27+F27)*$E$23+(G27+H27)*$G$23+(I27+J27)*$I$23+(K27+L27)*$K$23</f>
+      <c r="P27">
+        <f>(C27+D27)*$C$23+(E27+F27)*$E$23+(G27+H27)*$G$23+(I27+J27)*$I$23+(K27+L27)*$K$23</f>
         <v>415</v>
       </c>
-      <c r="O27" s="4">
-        <f t="shared" ref="O27:O31" si="3">M27-N27</f>
+      <c r="Q27" s="4">
+        <f t="shared" ref="Q27:Q31" si="1">O27-P27</f>
         <v>-20</v>
       </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -982,23 +1016,23 @@
       <c r="L28">
         <v>-1</v>
       </c>
-      <c r="M28">
+      <c r="O28">
+        <f>C28*$C$23+E28*$E$23+G28*$G$23+I28*$I$23+K28*$K$23</f>
+        <v>255</v>
+      </c>
+      <c r="P28">
+        <f>(C28+D28)*$C$23+(E28+F28)*$E$23+(G28+H28)*$G$23+(I28+J28)*$I$23+(K28+L28)*$K$23</f>
+        <v>210</v>
+      </c>
+      <c r="Q28" s="4">
         <f t="shared" si="1"/>
-        <v>255</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="O28" s="4">
-        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>5</v>
       </c>
@@ -1032,23 +1066,23 @@
       <c r="L29">
         <v>0</v>
       </c>
-      <c r="M29">
+      <c r="O29">
+        <f>C29*$C$23+E29*$E$23+G29*$G$23+I29*$I$23+K29*$K$23</f>
+        <v>245</v>
+      </c>
+      <c r="P29">
+        <f>(C29+D29)*$C$23+(E29+F29)*$E$23+(G29+H29)*$G$23+(I29+J29)*$I$23+(K29+L29)*$K$23</f>
+        <v>210</v>
+      </c>
+      <c r="Q29" s="4">
         <f t="shared" si="1"/>
-        <v>245</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="O29" s="4">
-        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>1</v>
       </c>
@@ -1082,23 +1116,23 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="M30">
+      <c r="O30">
+        <f>C30*$C$23+E30*$E$23+G30*$G$23+I30*$I$23+K30*$K$23</f>
+        <v>3836</v>
+      </c>
+      <c r="P30">
+        <f>(C30+D30)*$C$23+(E30+F30)*$E$23+(G30+H30)*$G$23+(I30+J30)*$I$23+(K30+L30)*$K$23</f>
+        <v>3923</v>
+      </c>
+      <c r="Q30" s="4">
         <f t="shared" si="1"/>
-        <v>3836</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="2"/>
-        <v>3923</v>
-      </c>
-      <c r="O30" s="4">
-        <f t="shared" si="3"/>
         <v>-87</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>20</v>
       </c>
@@ -1132,74 +1166,756 @@
       <c r="L31">
         <v>0</v>
       </c>
-      <c r="M31">
+      <c r="O31">
+        <f>C31*$C$23+E31*$E$23+G31*$G$23+I31*$I$23+K31*$K$23</f>
+        <v>60</v>
+      </c>
+      <c r="P31">
+        <f>(C31+D31)*$C$23+(E31+F31)*$E$23+(G31+H31)*$G$23+(I31+J31)*$I$23+(K31+L31)*$K$23</f>
+        <v>15</v>
+      </c>
+      <c r="Q31" s="4">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="N31">
+        <v>45</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" ref="C32:L32" si="2">SUM(C26:C31)</f>
+        <v>10</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="O32">
+        <f>SUM(O26:O31)</f>
+        <v>4981</v>
+      </c>
+      <c r="P32">
+        <f>SUM(P26:P31)</f>
+        <v>4918</v>
+      </c>
+      <c r="Q32" s="4">
+        <f>SUM(Q26:Q31)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N34" t="s">
+        <v>10</v>
+      </c>
+      <c r="O34" t="s">
+        <v>33</v>
+      </c>
+      <c r="P34" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f>C35*$C$23+E35*$E$23+G35*$G$23+I35*$I$23+K35*$K$23+M35*$M$23</f>
+        <v>75</v>
+      </c>
+      <c r="P35">
+        <f>(C35+D35)*$C$23+(E35+F35)*$E$23+(G35+H35)*$G$23+(I35+J35)*$I$23+(K35+L35)*$K$23+(M35+N35)*$M$23</f>
+        <v>105</v>
+      </c>
+      <c r="Q35" s="4">
+        <f>O35-P35</f>
+        <v>-30</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>-3</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>16</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ref="O36:O45" si="3">C36*$C$23+E36*$E$23+G36*$G$23+I36*$I$23+K36*$K$23+M36*$M$23</f>
+        <v>372</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ref="P36:P44" si="4">(C36+D36)*$C$23+(E36+F36)*$E$23+(G36+H36)*$G$23+(I36+J36)*$I$23+(K36+L36)*$K$23+(M36+N36)*$M$23</f>
+        <v>321</v>
+      </c>
+      <c r="Q36" s="4">
+        <f t="shared" ref="Q36:Q45" si="5">O36-P36</f>
+        <v>51</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>8</v>
+      </c>
+      <c r="L37">
+        <v>-4</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="Q37" s="4">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>-1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="Q38" s="4">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>-2</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>324</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>325</v>
+      </c>
+      <c r="Q39" s="4">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>90</v>
+      </c>
+      <c r="F40">
+        <v>-2</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>19</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>2100</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>2341</v>
+      </c>
+      <c r="Q40" s="4">
+        <f t="shared" si="5"/>
+        <v>-241</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="O31" s="4">
+      <c r="Q41" s="4">
+        <f t="shared" si="5"/>
+        <v>-15</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>-3</v>
+      </c>
+      <c r="E42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42">
+        <v>-3</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
         <f t="shared" si="3"/>
+        <v>272</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="Q42" s="4">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>132</v>
+      </c>
+      <c r="N43">
+        <v>-32</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="3"/>
+        <v>1980</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>1500</v>
+      </c>
+      <c r="Q43" s="4">
+        <f t="shared" si="5"/>
+        <v>480</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>45</v>
       </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <f t="shared" ref="C32:O32" si="4">SUM(C26:C31)</f>
-        <v>10</v>
-      </c>
-      <c r="D32">
+      <c r="J44">
+        <v>-10</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="3"/>
+        <v>675</v>
+      </c>
+      <c r="P44">
         <f t="shared" si="4"/>
+        <v>525</v>
+      </c>
+      <c r="Q44" s="4">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>SUM(C35:C44)</f>
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <f>SUM(D35:D44)</f>
         <v>-3</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="4"/>
-        <v>143</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="4"/>
-        <v>24</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="4"/>
+      <c r="E45">
+        <f>SUM(E35:E44)</f>
+        <v>114</v>
+      </c>
+      <c r="F45">
+        <f>SUM(F35:F44)</f>
         <v>-7</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="4"/>
-        <v>49</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="4"/>
+      <c r="G45">
+        <f>SUM(G35:G44)</f>
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <f>SUM(H35:H44)</f>
         <v>-1</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="4"/>
-        <v>4981</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="4"/>
-        <v>4918</v>
-      </c>
-      <c r="O32" s="4">
-        <f t="shared" si="4"/>
-        <v>63</v>
+      <c r="I45">
+        <f>SUM(I35:I44)</f>
+        <v>81</v>
+      </c>
+      <c r="J45">
+        <f>SUM(J35:J44)</f>
+        <v>15</v>
+      </c>
+      <c r="K45">
+        <f>SUM(K35:K44)</f>
+        <v>8</v>
+      </c>
+      <c r="L45">
+        <f>SUM(L35:L44)</f>
+        <v>-4</v>
+      </c>
+      <c r="M45">
+        <f>SUM(M35:M44)</f>
+        <v>132</v>
+      </c>
+      <c r="N45">
+        <f>SUM(N35:N44)</f>
+        <v>-32</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="3"/>
+        <v>6158</v>
+      </c>
+      <c r="P45">
+        <f>SUM(P35:P44)</f>
+        <v>5544</v>
+      </c>
+      <c r="Q45" s="4">
+        <f t="shared" si="5"/>
+        <v>614</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f>SUM(C45,E45,G45,I45,K45,M45)</f>
+        <v>345</v>
+      </c>
+      <c r="D46">
+        <f>SUM(C45:N45)</f>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato BV e SV
Aggiornato BV e SV per l'ultima prefase RA
</commit_message>
<xml_diff>
--- a/SWE/Documentazione/Piano_di_Progetto/file sorgenti/BVSV.xlsx
+++ b/SWE/Documentazione/Piano_di_Progetto/file sorgenti/BVSV.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
   <si>
     <t>norme di progetto</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>def prod</t>
+  </si>
+  <si>
+    <t>Preparazione collaudo</t>
+  </si>
+  <si>
+    <t>Collaudo</t>
   </si>
 </sst>
 </file>
@@ -202,10 +208,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R46"/>
+  <dimension ref="B2:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="D48" workbookViewId="0">
+      <selection activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,27 +813,27 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6" t="s">
+      <c r="J24" s="7"/>
+      <c r="K24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="7" t="s">
+      <c r="L24" s="7"/>
+      <c r="M24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="O24" t="s">
@@ -917,11 +923,11 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <f>C26*$C$23+E26*$E$23+G26*$G$23+I26*$I$23+K26*$K$23</f>
+        <f t="shared" ref="O26:O31" si="1">C26*$C$23+E26*$E$23+G26*$G$23+I26*$I$23+K26*$K$23</f>
         <v>190</v>
       </c>
       <c r="P26">
-        <f>(C26+D26)*$C$23+(E26+F26)*$E$23+(G26+H26)*$G$23+(I26+J26)*$I$23+(K26+L26)*$K$23</f>
+        <f t="shared" ref="P26:P31" si="2">(C26+D26)*$C$23+(E26+F26)*$E$23+(G26+H26)*$G$23+(I26+J26)*$I$23+(K26+L26)*$K$23</f>
         <v>145</v>
       </c>
       <c r="Q26" s="4">
@@ -967,15 +973,15 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <f>C27*$C$23+E27*$E$23+G27*$G$23+I27*$I$23+K27*$K$23</f>
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
       <c r="P27">
-        <f>(C27+D27)*$C$23+(E27+F27)*$E$23+(G27+H27)*$G$23+(I27+J27)*$I$23+(K27+L27)*$K$23</f>
+        <f t="shared" si="2"/>
         <v>415</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" ref="Q27:Q31" si="1">O27-P27</f>
+        <f t="shared" ref="Q27:Q31" si="3">O27-P27</f>
         <v>-20</v>
       </c>
       <c r="R27">
@@ -1017,15 +1023,15 @@
         <v>-1</v>
       </c>
       <c r="O28">
-        <f>C28*$C$23+E28*$E$23+G28*$G$23+I28*$I$23+K28*$K$23</f>
+        <f t="shared" si="1"/>
         <v>255</v>
       </c>
       <c r="P28">
-        <f>(C28+D28)*$C$23+(E28+F28)*$E$23+(G28+H28)*$G$23+(I28+J28)*$I$23+(K28+L28)*$K$23</f>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="Q28" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="R28">
@@ -1067,15 +1073,15 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <f>C29*$C$23+E29*$E$23+G29*$G$23+I29*$I$23+K29*$K$23</f>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
       <c r="P29">
-        <f>(C29+D29)*$C$23+(E29+F29)*$E$23+(G29+H29)*$G$23+(I29+J29)*$I$23+(K29+L29)*$K$23</f>
+        <f t="shared" si="2"/>
         <v>210</v>
       </c>
       <c r="Q29" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="R29">
@@ -1117,15 +1123,15 @@
         <v>0</v>
       </c>
       <c r="O30">
-        <f>C30*$C$23+E30*$E$23+G30*$G$23+I30*$I$23+K30*$K$23</f>
+        <f t="shared" si="1"/>
         <v>3836</v>
       </c>
       <c r="P30">
-        <f>(C30+D30)*$C$23+(E30+F30)*$E$23+(G30+H30)*$G$23+(I30+J30)*$I$23+(K30+L30)*$K$23</f>
+        <f t="shared" si="2"/>
         <v>3923</v>
       </c>
       <c r="Q30" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-87</v>
       </c>
       <c r="R30">
@@ -1167,15 +1173,15 @@
         <v>0</v>
       </c>
       <c r="O31">
-        <f>C31*$C$23+E31*$E$23+G31*$G$23+I31*$I$23+K31*$K$23</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="P31">
-        <f>(C31+D31)*$C$23+(E31+F31)*$E$23+(G31+H31)*$G$23+(I31+J31)*$I$23+(K31+L31)*$K$23</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="Q31" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="R31">
@@ -1184,43 +1190,43 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C32">
-        <f t="shared" ref="C32:L32" si="2">SUM(C26:C31)</f>
+        <f t="shared" ref="C32:L32" si="4">SUM(C26:C31)</f>
         <v>10</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>143</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-7</v>
       </c>
       <c r="I32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="J32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="L32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="O32">
@@ -1383,15 +1389,15 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36:O45" si="3">C36*$C$23+E36*$E$23+G36*$G$23+I36*$I$23+K36*$K$23+M36*$M$23</f>
+        <f t="shared" ref="O36:O45" si="5">C36*$C$23+E36*$E$23+G36*$G$23+I36*$I$23+K36*$K$23+M36*$M$23</f>
         <v>372</v>
       </c>
       <c r="P36">
-        <f t="shared" ref="P36:P44" si="4">(C36+D36)*$C$23+(E36+F36)*$E$23+(G36+H36)*$G$23+(I36+J36)*$I$23+(K36+L36)*$K$23+(M36+N36)*$M$23</f>
+        <f t="shared" ref="P36:P44" si="6">(C36+D36)*$C$23+(E36+F36)*$E$23+(G36+H36)*$G$23+(I36+J36)*$I$23+(K36+L36)*$K$23+(M36+N36)*$M$23</f>
         <v>321</v>
       </c>
       <c r="Q36" s="4">
-        <f t="shared" ref="Q36:Q45" si="5">O36-P36</f>
+        <f t="shared" ref="Q36:Q45" si="7">O36-P36</f>
         <v>51</v>
       </c>
       <c r="R36">
@@ -1439,15 +1445,15 @@
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="P37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="Q37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
       <c r="R37">
@@ -1495,15 +1501,15 @@
         <v>0</v>
       </c>
       <c r="O38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="P38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="Q38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
       <c r="R38">
@@ -1551,15 +1557,15 @@
         <v>0</v>
       </c>
       <c r="O39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>324</v>
       </c>
       <c r="P39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>325</v>
       </c>
       <c r="Q39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="R39">
@@ -1607,15 +1613,15 @@
         <v>0</v>
       </c>
       <c r="O40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2100</v>
       </c>
       <c r="P40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2341</v>
       </c>
       <c r="Q40" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-241</v>
       </c>
       <c r="R40">
@@ -1663,15 +1669,15 @@
         <v>0</v>
       </c>
       <c r="O41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="Q41" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-15</v>
       </c>
       <c r="R41">
@@ -1719,15 +1725,15 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>272</v>
       </c>
       <c r="P42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>167</v>
       </c>
       <c r="Q42" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>105</v>
       </c>
       <c r="R42">
@@ -1775,15 +1781,15 @@
         <v>-32</v>
       </c>
       <c r="O43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
       <c r="P43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="Q43" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>480</v>
       </c>
       <c r="R43">
@@ -1831,15 +1837,15 @@
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>675</v>
       </c>
       <c r="P44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>525</v>
       </c>
       <c r="Q44" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="R44">
@@ -1848,55 +1854,55 @@
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C45">
-        <f>SUM(C35:C44)</f>
+        <f t="shared" ref="C45:N45" si="8">SUM(C35:C44)</f>
         <v>7</v>
       </c>
       <c r="D45">
-        <f>SUM(D35:D44)</f>
+        <f t="shared" si="8"/>
         <v>-3</v>
       </c>
       <c r="E45">
-        <f>SUM(E35:E44)</f>
+        <f t="shared" si="8"/>
         <v>114</v>
       </c>
       <c r="F45">
-        <f>SUM(F35:F44)</f>
+        <f t="shared" si="8"/>
         <v>-7</v>
       </c>
       <c r="G45">
-        <f>SUM(G35:G44)</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H45">
-        <f>SUM(H35:H44)</f>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="I45">
-        <f>SUM(I35:I44)</f>
+        <f t="shared" si="8"/>
         <v>81</v>
       </c>
       <c r="J45">
-        <f>SUM(J35:J44)</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="K45">
-        <f>SUM(K35:K44)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="L45">
-        <f>SUM(L35:L44)</f>
+        <f t="shared" si="8"/>
         <v>-4</v>
       </c>
       <c r="M45">
-        <f>SUM(M35:M44)</f>
+        <f t="shared" si="8"/>
         <v>132</v>
       </c>
       <c r="N45">
-        <f>SUM(N35:N44)</f>
+        <f t="shared" si="8"/>
         <v>-32</v>
       </c>
       <c r="O45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6158</v>
       </c>
       <c r="P45">
@@ -1904,7 +1910,7 @@
         <v>5544</v>
       </c>
       <c r="Q45" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>614</v>
       </c>
     </row>
@@ -1916,6 +1922,803 @@
       <c r="D46">
         <f>SUM(C45:N45)</f>
         <v>313</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" t="s">
+        <v>10</v>
+      </c>
+      <c r="M49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R49" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>-1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <f>C50*$C$23+E50*$E$23+G50*$G$23+I50*$I$23+K50*$K$23+M50*$M$23</f>
+        <v>95</v>
+      </c>
+      <c r="P50">
+        <f>(C50+D50)*$C$23+(E50+F50)*$E$23+(G50+H50)*$G$23+(I50+J50)*$I$23+(K50+L50)*$K$23+(M50+N50)*$M$23</f>
+        <v>75</v>
+      </c>
+      <c r="Q50" s="4">
+        <f>O50-P50</f>
+        <v>20</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>31</v>
+      </c>
+      <c r="J51">
+        <v>-3</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <f t="shared" ref="O51:O62" si="9">C51*$C$23+E51*$E$23+G51*$G$23+I51*$I$23+K51*$K$23+M51*$M$23</f>
+        <v>465</v>
+      </c>
+      <c r="P51">
+        <f t="shared" ref="P51:P61" si="10">(C51+D51)*$C$23+(E51+F51)*$E$23+(G51+H51)*$G$23+(I51+J51)*$I$23+(K51+L51)*$K$23+(M51+N51)*$M$23</f>
+        <v>420</v>
+      </c>
+      <c r="Q51" s="4">
+        <f t="shared" ref="Q51:Q62" si="11">O51-P51</f>
+        <v>45</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>2</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="9"/>
+        <v>75</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="Q52" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="10"/>
+        <v>130</v>
+      </c>
+      <c r="Q53" s="4">
+        <f t="shared" si="11"/>
+        <v>-130</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>15</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="9"/>
+        <v>390</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="10"/>
+        <v>390</v>
+      </c>
+      <c r="Q54" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>15</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="9"/>
+        <v>390</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="10"/>
+        <v>390</v>
+      </c>
+      <c r="Q55" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="Q56" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>6</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>10</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="9"/>
+        <v>412</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="10"/>
+        <v>412</v>
+      </c>
+      <c r="Q57" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>2</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="Q58" s="4">
+        <f t="shared" si="11"/>
+        <v>-30</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="Q59" s="4">
+        <f t="shared" si="11"/>
+        <v>-15</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="9"/>
+        <v>160</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="10"/>
+        <v>160</v>
+      </c>
+      <c r="Q60" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>24</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>20</v>
+      </c>
+      <c r="N61">
+        <v>-2</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="9"/>
+        <v>660</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="10"/>
+        <v>630</v>
+      </c>
+      <c r="Q61" s="4">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f>SUM(C50:C61)</f>
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <f>SUM(D50:D61)</f>
+        <v>-1</v>
+      </c>
+      <c r="E62">
+        <f>SUM(E50:E61)</f>
+        <v>36</v>
+      </c>
+      <c r="F62">
+        <f>SUM(F50:F61)</f>
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f>SUM(G50:G61)</f>
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <f t="shared" ref="H62" si="12">SUM(H50:H59)</f>
+        <v>4</v>
+      </c>
+      <c r="I62">
+        <f>SUM(I50:I61)</f>
+        <v>72</v>
+      </c>
+      <c r="J62">
+        <f t="shared" ref="J62" si="13">SUM(J50:J59)</f>
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <f>SUM(K50:K61)</f>
+        <v>6</v>
+      </c>
+      <c r="L62">
+        <f>SUM(L50:L61)</f>
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <f>SUM(M50:M61)</f>
+        <v>30</v>
+      </c>
+      <c r="N62">
+        <f>SUM(N50:N61)</f>
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="9"/>
+        <v>2662</v>
+      </c>
+      <c r="P62">
+        <f>SUM(P50:P61)</f>
+        <v>2742</v>
+      </c>
+      <c r="Q62" s="4">
+        <f t="shared" si="11"/>
+        <v>-80</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f>SUM(C62,E62,G62,I62,K62,M62)</f>
+        <v>152</v>
+      </c>
+      <c r="D63">
+        <f>SUM(C62:N62)</f>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +2730,7 @@
     <mergeCell ref="K24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>